<commit_message>
[0.3.3.0] sum table done
</commit_message>
<xml_diff>
--- a/IRCS2-devbuild/source/test.xlsx
+++ b/IRCS2-devbuild/source/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="491">
   <si>
     <t>Items</t>
   </si>
@@ -1479,6 +1479,15 @@
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>UL_IDR</t>
+  </si>
+  <si>
+    <t>UL_USD</t>
   </si>
 </sst>
 </file>
@@ -13294,17 +13303,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:S3"/>
+  <dimension ref="B2:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="18" width="14.7109375" customWidth="1"/>
-    <col min="19" max="19" width="23.7109375" customWidth="1"/>
+    <col min="3" max="18" width="23.7109375" customWidth="1"/>
+    <col min="19" max="19" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:19">
+    <row r="2" spans="2:19">
+      <c r="B2" s="9" t="s">
+        <v>488</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
@@ -13333,7 +13345,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="3:19">
+    <row r="3" spans="2:19">
+      <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
@@ -13384,14 +13397,134 @@
       </c>
       <c r="S3" s="9"/>
     </row>
+    <row r="4" spans="2:19">
+      <c r="B4" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="C4" s="4">
+        <v>692991</v>
+      </c>
+      <c r="D4" s="4">
+        <v>11805853591983.16</v>
+      </c>
+      <c r="E4" s="4">
+        <v>217697314758240.2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>13875610295239.78</v>
+      </c>
+      <c r="G4" s="4">
+        <v>696400</v>
+      </c>
+      <c r="H4" s="4">
+        <v>11923781838617.36</v>
+      </c>
+      <c r="I4" s="4">
+        <v>218913632365850.2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>13917077488107.32</v>
+      </c>
+      <c r="K4" s="4">
+        <v>-3409</v>
+      </c>
+      <c r="L4" s="4">
+        <v>-117928246634.2052</v>
+      </c>
+      <c r="M4" s="4">
+        <v>-1216317607610</v>
+      </c>
+      <c r="N4" s="4">
+        <v>-41467192867.53465</v>
+      </c>
+      <c r="O4" s="8">
+        <f>IFERROR(round(K4/G4 * 100, 1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="8">
+        <f>IFERROR(round(L4/H4 * 100, 1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
+        <f>IFERROR(round(M4/I4 * 100, 1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="8">
+        <f>IFERROR(round(N4/J4 * 100, 1),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19">
+      <c r="B5" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="C5" s="4">
+        <v>9222</v>
+      </c>
+      <c r="D5" s="4">
+        <v>73416089.39</v>
+      </c>
+      <c r="E5" s="4">
+        <v>875620109.1160001</v>
+      </c>
+      <c r="F5" s="4">
+        <v>287925652.9790439</v>
+      </c>
+      <c r="G5" s="4">
+        <v>9222</v>
+      </c>
+      <c r="H5" s="4">
+        <v>73416089.39</v>
+      </c>
+      <c r="I5" s="4">
+        <v>875620109.1160001</v>
+      </c>
+      <c r="J5" s="4">
+        <v>287925652.6236017</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.3554421301923867</v>
+      </c>
+      <c r="O5" s="8">
+        <f>IFERROR(round(K5/G5 * 100, 1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="8">
+        <f>IFERROR(round(L5/H5 * 100, 1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="8">
+        <f>IFERROR(round(M5/I5 * 100, 1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="8">
+        <f>IFERROR(round(N5/J5 * 100, 1),0)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:S3"/>
+    <mergeCell ref="B2:B3"/>
   </mergeCells>
+  <conditionalFormatting sqref="O4:R999">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[0.3.3.1] fixed UL calculation
</commit_message>
<xml_diff>
--- a/IRCS2-devbuild/source/test.xlsx
+++ b/IRCS2-devbuild/source/test.xlsx
@@ -2042,16 +2042,20 @@
         <v>-41467192867.17773</v>
       </c>
       <c r="Q3" s="5">
-        <v>-0.0006649683819707874</v>
+        <f>IFERROR(round(M4/I4 * 100, 1),0)</f>
+        <v>0</v>
       </c>
       <c r="R3" s="5">
-        <v>-2.269549213464004E-12</v>
+        <f>IFERROR(round(N4/J4 * 100, 1),0)</f>
+        <v>0</v>
       </c>
       <c r="S3" s="5">
-        <v>-4.238386091373726E-11</v>
+        <f>IFERROR(round(O4/K4 * 100, 1),0)</f>
+        <v>0</v>
       </c>
       <c r="T3" s="5">
-        <v>-3.468534131063111E-11</v>
+        <f>IFERROR(round(P4/L4 * 100, 1),0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:22">

</xml_diff>

<commit_message>
[0.4.2.7] major trad integration
</commit_message>
<xml_diff>
--- a/IRCS2-devbuild/source/test.xlsx
+++ b/IRCS2-devbuild/source/test.xlsx
@@ -13422,26 +13422,14 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="4">
-        <v>467368</v>
-      </c>
-      <c r="J3" s="4">
-        <v>95679515934153</v>
-      </c>
-      <c r="K3" s="4">
-        <v>4308204442004.65</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
       <c r="M3" s="4">
-        <v>3402</v>
+        <v>3148</v>
       </c>
       <c r="N3" s="4">
-        <v>3772969980932.797</v>
+        <v>3625443648632.797</v>
       </c>
       <c r="O3" s="4">
-        <v>117057845167.0332</v>
+        <v>109739235167.0332</v>
       </c>
       <c r="P3" s="4">
         <v>0</v>
@@ -13451,15 +13439,111 @@
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E4" s="4">
+        <v>470516</v>
+      </c>
+      <c r="F4" s="4">
+        <v>99304959582785.8</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4417943677171.684</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>467368</v>
+      </c>
+      <c r="J4" s="4">
+        <v>95679515934153</v>
+      </c>
+      <c r="K4" s="4">
+        <v>4308204442004.65</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:21">
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E5" s="6">
+        <f>E3-E4</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <f>F3-F4</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <f>G3-G4</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <f>H3-H4</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <f>I3-I4</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <f>J3-J4</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <f>K3-K4</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <f>L3-L4</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <f>M3-M4</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <f>N3-N4</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
+        <f>O3-O4</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
+        <f>P3-P4</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:21">
       <c r="D6" s="9" t="s">
         <v>488</v>
+      </c>
+      <c r="E6" s="4">
+        <v>470516</v>
+      </c>
+      <c r="F6" s="4">
+        <v>99304959582785.8</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4417943677171.684</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>467368</v>
+      </c>
+      <c r="J6" s="4">
+        <v>95679515934153</v>
+      </c>
+      <c r="K6" s="4">
+        <v>4308204442004.65</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:21">

</xml_diff>